<commit_message>
cleaned up uneeded files
</commit_message>
<xml_diff>
--- a/Output/future_adr.xlsx
+++ b/Output/future_adr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Jun</t>
+          <t>Aug</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -561,373 +561,373 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>41.03178571428571</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>43.20724137931035</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>43.35515151515152</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>67.57973684210526</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>64.7193023255814</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>45.30756756756757</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>41.7053125</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>41.0888</v>
       </c>
       <c r="Q2" t="n">
-        <v>57.12686274509804</v>
+        <v>41.54130434782609</v>
       </c>
       <c r="R2" t="n">
-        <v>53.48976744186047</v>
+        <v>46.15476190476191</v>
       </c>
       <c r="S2" t="n">
-        <v>44.85651162790698</v>
+        <v>53.79944444444445</v>
       </c>
       <c r="T2" t="n">
-        <v>38.98</v>
+        <v>52.6635</v>
       </c>
       <c r="U2" t="n">
-        <v>41.22586206896552</v>
+        <v>42.33071428571429</v>
       </c>
       <c r="V2" t="n">
-        <v>43.18111111111111</v>
+        <v>37.64</v>
       </c>
       <c r="W2" t="n">
-        <v>45.0137037037037</v>
+        <v>37.71541666666666</v>
       </c>
       <c r="X2" t="n">
-        <v>50.32875</v>
+        <v>37.19391304347826</v>
       </c>
       <c r="Y2" t="n">
-        <v>58.60969696969697</v>
+        <v>37.671</v>
       </c>
       <c r="Z2" t="n">
-        <v>42.09391304347826</v>
+        <v>54.76111111111111</v>
       </c>
       <c r="AA2" t="n">
-        <v>43.99230769230769</v>
+        <v>60.02206896551724</v>
       </c>
       <c r="AB2" t="n">
-        <v>44.03083333333333</v>
+        <v>58.6721052631579</v>
       </c>
       <c r="AC2" t="n">
-        <v>42.35</v>
+        <v>61.83333333333334</v>
       </c>
       <c r="AD2" t="n">
-        <v>45.76214285714286</v>
+        <v>61.21875</v>
       </c>
       <c r="AE2" t="n">
-        <v>55.305625</v>
+        <v>47.82727272727273</v>
       </c>
       <c r="AF2" t="n">
-        <v>0</v>
+        <v>52.17368421052631</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Jul</t>
+          <t>Sep</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>51.863125</v>
+        <v>61.82958333333334</v>
       </c>
       <c r="C3" t="n">
-        <v>42.11736842105263</v>
+        <v>60.62612903225807</v>
       </c>
       <c r="D3" t="n">
-        <v>39.55636363636363</v>
+        <v>52.075</v>
       </c>
       <c r="E3" t="n">
-        <v>41.675</v>
+        <v>44.89909090909091</v>
       </c>
       <c r="F3" t="n">
-        <v>40.2584375</v>
+        <v>43.16090909090909</v>
       </c>
       <c r="G3" t="n">
-        <v>42.74632653061225</v>
+        <v>44.332</v>
       </c>
       <c r="H3" t="n">
-        <v>50.75584905660377</v>
+        <v>45.7125</v>
       </c>
       <c r="I3" t="n">
-        <v>51.62982142857143</v>
+        <v>55.50894736842105</v>
       </c>
       <c r="J3" t="n">
-        <v>44.84769230769231</v>
+        <v>49.98708333333334</v>
       </c>
       <c r="K3" t="n">
-        <v>38.03428571428572</v>
+        <v>48.82761904761905</v>
       </c>
       <c r="L3" t="n">
-        <v>41.78</v>
+        <v>46.9078947368421</v>
       </c>
       <c r="M3" t="n">
-        <v>38.00714285714286</v>
+        <v>45.17173913043479</v>
       </c>
       <c r="N3" t="n">
-        <v>38.68125</v>
+        <v>45.14346153846154</v>
       </c>
       <c r="O3" t="n">
-        <v>52.44733333333333</v>
+        <v>41.001</v>
       </c>
       <c r="P3" t="n">
-        <v>52.09666666666667</v>
+        <v>57.71897435897436</v>
       </c>
       <c r="Q3" t="n">
-        <v>42.56666666666667</v>
+        <v>56.03558823529412</v>
       </c>
       <c r="R3" t="n">
-        <v>39</v>
+        <v>40.24842105263158</v>
       </c>
       <c r="S3" t="n">
-        <v>44.92</v>
+        <v>46.1605</v>
       </c>
       <c r="T3" t="n">
-        <v>52.879</v>
+        <v>49.85333333333334</v>
       </c>
       <c r="U3" t="n">
-        <v>54.57375</v>
+        <v>49.1325</v>
       </c>
       <c r="V3" t="n">
-        <v>48.48333333333333</v>
+        <v>46.5945</v>
       </c>
       <c r="W3" t="n">
-        <v>50.75875</v>
+        <v>51.443</v>
       </c>
       <c r="X3" t="n">
-        <v>40.69625</v>
+        <v>46.95647058823529</v>
       </c>
       <c r="Y3" t="n">
-        <v>35.4625</v>
+        <v>40.33214285714286</v>
       </c>
       <c r="Z3" t="n">
-        <v>36.528</v>
+        <v>35.83461538461539</v>
       </c>
       <c r="AA3" t="n">
-        <v>45.09384615384616</v>
+        <v>36.08846153846154</v>
       </c>
       <c r="AB3" t="n">
-        <v>47.35096774193548</v>
+        <v>43.75</v>
       </c>
       <c r="AC3" t="n">
-        <v>59.77764705882353</v>
+        <v>47.32333333333334</v>
       </c>
       <c r="AD3" t="n">
-        <v>60.79941176470588</v>
+        <v>73.20588235294117</v>
       </c>
       <c r="AE3" t="n">
-        <v>53.63285714285714</v>
+        <v>66.01590909090909</v>
       </c>
       <c r="AF3" t="n">
-        <v>49.654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Aug</t>
+          <t>Oct</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>71.7625</v>
+        <v>116</v>
       </c>
       <c r="C4" t="n">
-        <v>57.36666666666667</v>
+        <v>124.5</v>
       </c>
       <c r="D4" t="n">
-        <v>51.7</v>
+        <v>124.5</v>
       </c>
       <c r="E4" t="n">
-        <v>48.47333333333334</v>
+        <v>41</v>
       </c>
       <c r="F4" t="n">
-        <v>48.47333333333334</v>
+        <v>73</v>
       </c>
       <c r="G4" t="n">
+        <v>104.2173913043478</v>
+      </c>
+      <c r="H4" t="n">
+        <v>105.2727272727273</v>
+      </c>
+      <c r="I4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="J4" t="n">
+        <v>39.66666666666666</v>
+      </c>
+      <c r="K4" t="n">
+        <v>39.66666666666666</v>
+      </c>
+      <c r="L4" t="n">
+        <v>39.66666666666666</v>
+      </c>
+      <c r="M4" t="n">
+        <v>87.46153846153847</v>
+      </c>
+      <c r="N4" t="n">
+        <v>109.0869565217391</v>
+      </c>
+      <c r="O4" t="n">
+        <v>109.0869565217391</v>
+      </c>
+      <c r="P4" t="n">
+        <v>75.52380952380952</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>53.42857142857143</v>
+      </c>
+      <c r="R4" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="S4" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="T4" t="n">
+        <v>75.30434782608695</v>
+      </c>
+      <c r="U4" t="n">
+        <v>96.42307692307692</v>
+      </c>
+      <c r="V4" t="n">
+        <v>104.84</v>
+      </c>
+      <c r="W4" t="n">
+        <v>76.47619047619048</v>
+      </c>
+      <c r="X4" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="Y4" t="n">
         <v>41</v>
       </c>
-      <c r="H4" t="n">
-        <v>39</v>
-      </c>
-      <c r="I4" t="n">
-        <v>44.23333333333333</v>
-      </c>
-      <c r="J4" t="n">
-        <v>41.8625</v>
-      </c>
-      <c r="K4" t="n">
-        <v>38.82857142857143</v>
-      </c>
-      <c r="L4" t="n">
-        <v>85.53538461538461</v>
-      </c>
-      <c r="M4" t="n">
-        <v>80.42117647058822</v>
-      </c>
-      <c r="N4" t="n">
-        <v>43.68588235294118</v>
-      </c>
-      <c r="O4" t="n">
-        <v>44.00428571428571</v>
-      </c>
-      <c r="P4" t="n">
-        <v>44.06</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>46.59</v>
-      </c>
-      <c r="R4" t="n">
-        <v>56.25</v>
-      </c>
-      <c r="S4" t="n">
-        <v>56.09999999999999</v>
-      </c>
-      <c r="T4" t="n">
-        <v>49.86666666666667</v>
-      </c>
-      <c r="U4" t="n">
-        <v>34</v>
-      </c>
-      <c r="V4" t="n">
-        <v>36.17666666666667</v>
-      </c>
-      <c r="W4" t="n">
-        <v>38.296</v>
-      </c>
-      <c r="X4" t="n">
-        <v>37.496</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>38.22571428571428</v>
-      </c>
       <c r="Z4" t="n">
-        <v>46.67285714285714</v>
+        <v>49.25</v>
       </c>
       <c r="AA4" t="n">
-        <v>59.78727272727272</v>
+        <v>65.93333333333334</v>
       </c>
       <c r="AB4" t="n">
-        <v>67.86777777777777</v>
+        <v>87</v>
       </c>
       <c r="AC4" t="n">
-        <v>73.94166666666666</v>
+        <v>87</v>
       </c>
       <c r="AD4" t="n">
-        <v>99.21666666666665</v>
+        <v>58.66666666666666</v>
       </c>
       <c r="AE4" t="n">
-        <v>74.56666666666666</v>
+        <v>41</v>
       </c>
       <c r="AF4" t="n">
-        <v>49.3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Sep</t>
+          <t>Nov</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>56.79071428571429</v>
+        <v>41</v>
       </c>
       <c r="C5" t="n">
-        <v>61.78235294117647</v>
+        <v>62</v>
       </c>
       <c r="D5" t="n">
-        <v>53.56944444444444</v>
+        <v>81</v>
       </c>
       <c r="E5" t="n">
-        <v>45.57615384615384</v>
+        <v>81.2</v>
       </c>
       <c r="F5" t="n">
-        <v>48.2125</v>
+        <v>52</v>
       </c>
       <c r="G5" t="n">
-        <v>50.715</v>
+        <v>41</v>
       </c>
       <c r="H5" t="n">
-        <v>55.255</v>
+        <v>41</v>
       </c>
       <c r="I5" t="n">
-        <v>69.30454545454546</v>
+        <v>38</v>
       </c>
       <c r="J5" t="n">
-        <v>61.76230769230769</v>
+        <v>49.5</v>
       </c>
       <c r="K5" t="n">
-        <v>73.99285714285715</v>
+        <v>41</v>
       </c>
       <c r="L5" t="n">
-        <v>66.38571428571429</v>
+        <v>41</v>
       </c>
       <c r="M5" t="n">
-        <v>71.5</v>
+        <v>37</v>
       </c>
       <c r="N5" t="n">
-        <v>63.75375</v>
+        <v>35</v>
       </c>
       <c r="O5" t="n">
-        <v>55.86142857142857</v>
+        <v>35</v>
       </c>
       <c r="P5" t="n">
-        <v>85.63142857142857</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>85.63142857142857</v>
+        <v>37.775</v>
       </c>
       <c r="R5" t="n">
-        <v>40.45166666666667</v>
+        <v>45.6</v>
       </c>
       <c r="S5" t="n">
-        <v>43.94142857142857</v>
+        <v>47.16666666666666</v>
       </c>
       <c r="T5" t="n">
-        <v>47.79333333333333</v>
+        <v>34.53333333333333</v>
       </c>
       <c r="U5" t="n">
-        <v>41.91666666666666</v>
+        <v>29.84</v>
       </c>
       <c r="V5" t="n">
-        <v>45.52692307692308</v>
+        <v>33.33333333333334</v>
       </c>
       <c r="W5" t="n">
-        <v>55.27083333333334</v>
+        <v>35.5</v>
       </c>
       <c r="X5" t="n">
-        <v>49.40625</v>
+        <v>37.3925</v>
       </c>
       <c r="Y5" t="n">
-        <v>38.475</v>
+        <v>42.89000000000001</v>
       </c>
       <c r="Z5" t="n">
-        <v>36.03333333333333</v>
+        <v>43.2175</v>
       </c>
       <c r="AA5" t="n">
-        <v>36.03333333333333</v>
+        <v>37.95666666666667</v>
       </c>
       <c r="AB5" t="n">
-        <v>36.55</v>
+        <v>38.08</v>
       </c>
       <c r="AC5" t="n">
-        <v>77.59</v>
+        <v>37</v>
       </c>
       <c r="AD5" t="n">
-        <v>116.6</v>
+        <v>35.5</v>
       </c>
       <c r="AE5" t="n">
-        <v>86.86</v>
+        <v>37.35</v>
       </c>
       <c r="AF5" t="n">
         <v>0</v>
@@ -936,135 +936,135 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Oct</t>
+          <t>Dec</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>244</v>
+        <v>45.47333333333334</v>
       </c>
       <c r="C6" t="n">
-        <v>208</v>
+        <v>44</v>
       </c>
       <c r="D6" t="n">
-        <v>124.5</v>
+        <v>39</v>
       </c>
       <c r="E6" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F6" t="n">
-        <v>60.36363636363637</v>
+        <v>68</v>
       </c>
       <c r="G6" t="n">
-        <v>96.33333333333333</v>
+        <v>68</v>
       </c>
       <c r="H6" t="n">
-        <v>96.33333333333333</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>64.14285714285714</v>
+        <v>66</v>
       </c>
       <c r="J6" t="n">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="K6" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L6" t="n">
-        <v>41</v>
+        <v>26.78333333333333</v>
       </c>
       <c r="M6" t="n">
-        <v>76.375</v>
+        <v>26.78333333333333</v>
       </c>
       <c r="N6" t="n">
-        <v>95.375</v>
+        <v>24.74</v>
       </c>
       <c r="O6" t="n">
-        <v>95.375</v>
+        <v>39</v>
       </c>
       <c r="P6" t="n">
-        <v>66.84615384615384</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>41</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="T6" t="n">
-        <v>77.15789473684211</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="U6" t="n">
-        <v>104</v>
+        <v>39.26</v>
       </c>
       <c r="V6" t="n">
-        <v>108.0588235294118</v>
+        <v>39.125</v>
       </c>
       <c r="W6" t="n">
-        <v>84.07692307692308</v>
+        <v>43.125</v>
       </c>
       <c r="X6" t="n">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="Y6" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Z6" t="n">
-        <v>54.2</v>
+        <v>37</v>
       </c>
       <c r="AA6" t="n">
-        <v>65.83333333333333</v>
+        <v>37</v>
       </c>
       <c r="AB6" t="n">
-        <v>87.57142857142857</v>
+        <v>37</v>
       </c>
       <c r="AC6" t="n">
-        <v>87.57142857142857</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
-        <v>60.83333333333334</v>
+        <v>47</v>
       </c>
       <c r="AE6" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AF6" t="n">
-        <v>41</v>
+        <v>37.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Nov</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>41</v>
+        <v>36.8</v>
       </c>
       <c r="C7" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -1091,43 +1091,43 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>47.2</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>39</v>
+        <v>66.33333333333333</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>66.33333333333333</v>
       </c>
       <c r="V7" t="n">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="W7" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>37.435</v>
+        <v>37</v>
       </c>
       <c r="Y7" t="n">
-        <v>40.835</v>
+        <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>40.835</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>39.17</v>
+        <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>39.16</v>
+        <v>0</v>
       </c>
       <c r="AC7" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AD7" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="AF7" t="n">
         <v>0</v>
@@ -1136,14 +1136,14 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Dec</t>
+          <t>Feb</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>42.5</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -1161,19 +1161,19 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>37.4</v>
       </c>
       <c r="K8" t="n">
-        <v>39</v>
+        <v>37.4</v>
       </c>
       <c r="L8" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -1182,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>74.5</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
@@ -1200,95 +1200,95 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AC8" t="n">
         <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>Mar</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="E9" t="n">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="F9" t="n">
-        <v>47</v>
+        <v>189</v>
       </c>
       <c r="G9" t="n">
-        <v>47</v>
+        <v>121.5</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>87.33333333333333</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>87.33333333333333</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>62.33333333333334</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>47.75</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>81.5</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -1306,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
@@ -1327,9 +1327,309 @@
         <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AF9" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>52.225</v>
+      </c>
+      <c r="F10" t="n">
+        <v>76.6970588235294</v>
+      </c>
+      <c r="G10" t="n">
+        <v>82.5242105263158</v>
+      </c>
+      <c r="H10" t="n">
+        <v>72.56</v>
+      </c>
+      <c r="I10" t="n">
+        <v>61.6375</v>
+      </c>
+      <c r="J10" t="n">
+        <v>61.47692307692308</v>
+      </c>
+      <c r="K10" t="n">
+        <v>102.6666666666667</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>43</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>109.5</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>109.5</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated CB_API and Dash
</commit_message>
<xml_diff>
--- a/Output/future_adr.xlsx
+++ b/Output/future_adr.xlsx
@@ -609,19 +609,19 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>54.995625</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>67.40192307692307</v>
+        <v>66.19027777777778</v>
       </c>
       <c r="Z2" t="n">
-        <v>54.37355769230769</v>
+        <v>53.53392857142858</v>
       </c>
       <c r="AA2" t="n">
-        <v>55.73598214285714</v>
+        <v>55.15363175675675</v>
       </c>
       <c r="AB2" t="n">
-        <v>62.9790625</v>
+        <v>58.160625</v>
       </c>
       <c r="AC2" t="n">
         <v>34.95637499999999</v>
@@ -653,13 +653,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>50.76213662790698</v>
+        <v>49.41402925531915</v>
       </c>
       <c r="E3" t="n">
-        <v>51.52340425531915</v>
+        <v>50.22132352941176</v>
       </c>
       <c r="F3" t="n">
-        <v>40.60493951612903</v>
+        <v>40.38193359375</v>
       </c>
       <c r="G3" t="n">
         <v>43.7171875</v>
@@ -683,22 +683,22 @@
         <v>67.89930555555556</v>
       </c>
       <c r="N3" t="n">
-        <v>55.90745192307692</v>
+        <v>55.80778301886792</v>
       </c>
       <c r="O3" t="n">
+        <v>56.88100961538461</v>
+      </c>
+      <c r="P3" t="n">
         <v>57.00367647058824</v>
       </c>
-      <c r="P3" t="n">
-        <v>57.13124999999999</v>
-      </c>
       <c r="Q3" t="n">
-        <v>79.64923469387755</v>
+        <v>79.53749999999999</v>
       </c>
       <c r="R3" t="n">
-        <v>97.33695652173913</v>
+        <v>97.04122340425532</v>
       </c>
       <c r="S3" t="n">
-        <v>93.427734375</v>
+        <v>93.12499999999999</v>
       </c>
       <c r="T3" t="n">
         <v>74.78365384615384</v>
@@ -716,34 +716,34 @@
         <v>56.490234375</v>
       </c>
       <c r="Y3" t="n">
-        <v>76.98253676470588</v>
+        <v>75.4140625</v>
       </c>
       <c r="Z3" t="n">
-        <v>78.48656250000001</v>
+        <v>75.78323863636365</v>
       </c>
       <c r="AA3" t="n">
-        <v>46.66953125</v>
+        <v>46.03629807692307</v>
       </c>
       <c r="AB3" t="n">
-        <v>31.61071428571428</v>
+        <v>31.83579545454545</v>
       </c>
       <c r="AC3" t="n">
         <v>36.88124999999999</v>
       </c>
       <c r="AD3" t="n">
-        <v>32.05546875</v>
+        <v>32.32058823529412</v>
       </c>
       <c r="AE3" t="n">
-        <v>45.73014705882353</v>
+        <v>45.325</v>
       </c>
       <c r="AF3" t="n">
-        <v>52.24285714285715</v>
+        <v>51.93913043478261</v>
       </c>
       <c r="AG3" t="n">
-        <v>42.98112980769231</v>
+        <v>43.57790948275862</v>
       </c>
       <c r="AH3" t="n">
-        <v>40.22812499999999</v>
+        <v>40.37410714285714</v>
       </c>
     </row>
     <row r="4">
@@ -757,19 +757,19 @@
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>44.3535</v>
+        <v>44.16201923076923</v>
       </c>
       <c r="E4" t="n">
         <v>38.19508928571428</v>
       </c>
       <c r="F4" t="n">
-        <v>41.94866071428572</v>
+        <v>41.67732558139534</v>
       </c>
       <c r="G4" t="n">
         <v>46.52104591836735</v>
       </c>
       <c r="H4" t="n">
-        <v>99.74629934210527</v>
+        <v>99.328125</v>
       </c>
       <c r="I4" t="n">
         <v>100.7334603658537</v>
@@ -817,10 +817,10 @@
         <v>46.09553571428572</v>
       </c>
       <c r="X4" t="n">
-        <v>39.86116071428571</v>
+        <v>39.261328125</v>
       </c>
       <c r="Y4" t="n">
-        <v>39.409375</v>
+        <v>38.446875</v>
       </c>
       <c r="Z4" t="n">
         <v>45.59866071428571</v>
@@ -909,13 +909,13 @@
         <v>65.71875</v>
       </c>
       <c r="T5" t="n">
-        <v>71.81953125</v>
+        <v>72.01875</v>
       </c>
       <c r="U5" t="n">
-        <v>69.56875000000001</v>
+        <v>68.60937499999999</v>
       </c>
       <c r="V5" t="n">
-        <v>55.2359375</v>
+        <v>38.984375</v>
       </c>
       <c r="W5" t="n">
         <v>36.5625</v>

</xml_diff>